<commit_message>
nice progree on random walk
</commit_message>
<xml_diff>
--- a/tsfl_2s_factors_daily_correlation.xlsx
+++ b/tsfl_2s_factors_daily_correlation.xlsx
@@ -530,52 +530,52 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1653177332832542</v>
+        <v>-0.1652581622154127</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.002521174352252688</v>
+        <v>-0.002523758263964982</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0003069513591253482</v>
+        <v>0.0002931071949994339</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001119163857363431</v>
+        <v>0.001124234086298129</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.001277971394629365</v>
+        <v>-0.00127753765741268</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.0007965877032208406</v>
+        <v>-0.0007990859124778034</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001138456016208976</v>
+        <v>0.001177632623395438</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0004150461221734163</v>
+        <v>0.0004195049823813824</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.002190673373236816</v>
+        <v>-0.00219475635291615</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.001168230183307748</v>
+        <v>-0.001166882514834089</v>
       </c>
       <c r="M2" t="n">
-        <v>0.001626639367515433</v>
+        <v>0.001634561894822562</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0008292350778359623</v>
+        <v>0.0008368912573226979</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.001441381663814337</v>
+        <v>-0.001468032878502348</v>
       </c>
       <c r="P2" t="n">
-        <v>0.001236075115874026</v>
+        <v>0.001248231948587792</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.0001809993921905026</v>
+        <v>-0.0001451763067674667</v>
       </c>
       <c r="R2" t="n">
-        <v>0.002490200880877209</v>
+        <v>0.002522203803982969</v>
       </c>
     </row>
     <row r="3">
@@ -585,55 +585,55 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1653177332832542</v>
+        <v>-0.1652581622154127</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002368947849853727</v>
+        <v>0.002369369501396157</v>
       </c>
       <c r="E3" t="n">
-        <v>8.802648853724262e-05</v>
+        <v>8.467925534031512e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2843987337149366</v>
+        <v>0.2844015208501288</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0004854842542088133</v>
+        <v>-0.0004875614275482367</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0002284427686722433</v>
+        <v>-0.0002308575196248227</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0003264826249559733</v>
+        <v>0.0003402204221353358</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0001190255446989295</v>
+        <v>0.0001211958291220369</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0006282340144309354</v>
+        <v>-0.000634069503543657</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.0003350211614406856</v>
+        <v>-0.0003371146942535636</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0004664822206589636</v>
+        <v>0.0004722282032739412</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0002473712335797657</v>
+        <v>0.0002513753691377797</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.0006725001572570425</v>
+        <v>-0.000686895551804251</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0003441936607030431</v>
+        <v>0.0003503091363556556</v>
       </c>
       <c r="Q3" t="n">
-        <v>-8.598931052432631e-05</v>
+        <v>-6.915549790652933e-05</v>
       </c>
       <c r="R3" t="n">
-        <v>0.001249376620106088</v>
+        <v>0.001265568880261699</v>
       </c>
     </row>
     <row r="4">
@@ -643,55 +643,55 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.002521174352252688</v>
+        <v>-0.002523758263964982</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002368947849853727</v>
+        <v>0.002369369501396157</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1349543810557835</v>
+        <v>0.1349809246210455</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1579194644497394</v>
+        <v>0.157923111777737</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0004100052247146033</v>
+        <v>0.0004048714336955325</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0002345372470887257</v>
+        <v>0.0002323913823368846</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0003351926459486996</v>
+        <v>-0.0003424809134566106</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0001222009510255731</v>
+        <v>-0.0001220010780195644</v>
       </c>
       <c r="K4" t="n">
-        <v>0.000644994267613835</v>
+        <v>0.0006382823858887653</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0003439589765832899</v>
+        <v>0.0003393545505090623</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.0004789272012616987</v>
+        <v>-0.0004753657802256805</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0002559531140789645</v>
+        <v>-0.0002552659143308778</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0002627277026265624</v>
+        <v>0.0002627615482830759</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0003448736322703561</v>
+        <v>-0.0003439280965548492</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.049023167331969e-05</v>
+        <v>2.39965511444554e-05</v>
       </c>
       <c r="R4" t="n">
-        <v>0.2586872770139811</v>
+        <v>0.2585231779625458</v>
       </c>
     </row>
     <row r="5">
@@ -701,55 +701,55 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0003069513591253482</v>
+        <v>0.0002931071949994339</v>
       </c>
       <c r="C5" t="n">
-        <v>8.802648853724262e-05</v>
+        <v>8.467925534031512e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1349543810557835</v>
+        <v>0.1349809246210455</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.226230660336027</v>
+        <v>0.2261890848751147</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0001576883407345419</v>
+        <v>0.0001495056164569069</v>
       </c>
       <c r="H5" t="n">
-        <v>8.903136686902814e-05</v>
+        <v>8.451679271108418e-05</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0001272405974050862</v>
+        <v>-0.0001245544825252122</v>
       </c>
       <c r="J5" t="n">
-        <v>-4.638801656289278e-05</v>
+        <v>-4.436971680226623e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0002448426507142497</v>
+        <v>0.0002321324463804022</v>
       </c>
       <c r="L5" t="n">
-        <v>0.000130568334932927</v>
+        <v>0.0001234174775012411</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.000181802864527671</v>
+        <v>-0.0001728824481591328</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0001022687416452939</v>
+        <v>-9.817768454003779e-05</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0003191134297649877</v>
+        <v>0.0003146591035266696</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0001056255564091651</v>
+        <v>-9.939581574887584e-05</v>
       </c>
       <c r="Q5" t="n">
-        <v>3.100195286639313e-05</v>
+        <v>2.389315715687617e-05</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1147153398274242</v>
+        <v>0.1142621748737162</v>
       </c>
     </row>
     <row r="6">
@@ -759,55 +759,55 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001119163857363431</v>
+        <v>0.001124234086298129</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2843987337149366</v>
+        <v>0.2844015208501288</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1579194644497394</v>
+        <v>0.157923111777737</v>
       </c>
       <c r="E6" t="n">
-        <v>0.226230660336027</v>
+        <v>0.2261890848751147</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.2188914863222956</v>
+        <v>-0.218824225336559</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03485171557652254</v>
+        <v>0.03486044852935592</v>
       </c>
       <c r="I6" t="n">
-        <v>0.06358113438030931</v>
+        <v>0.06371089685032538</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2400588909222834</v>
+        <v>0.2400602062985029</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.2194922147890637</v>
+        <v>-0.2194358192293704</v>
       </c>
       <c r="L6" t="n">
-        <v>0.02393631303165519</v>
+        <v>0.02395877534143304</v>
       </c>
       <c r="M6" t="n">
-        <v>0.07430413120145614</v>
+        <v>0.07431340951733358</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4943070047759678</v>
+        <v>0.4941702061229365</v>
       </c>
       <c r="O6" t="n">
-        <v>0.08673829665631627</v>
+        <v>0.08661242330160181</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.01866525350856984</v>
+        <v>-0.01860508477477728</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.01034470413893863</v>
+        <v>0.01058778278023932</v>
       </c>
       <c r="R6" t="n">
-        <v>0.2958933948009917</v>
+        <v>0.295895750700426</v>
       </c>
     </row>
     <row r="7">
@@ -817,55 +817,55 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.001277971394629365</v>
+        <v>-0.00127753765741268</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0004854842542088133</v>
+        <v>-0.0004875614275482367</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004100052247146033</v>
+        <v>0.0004048714336955325</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0001576883407345419</v>
+        <v>0.0001495056164569069</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.2188914863222956</v>
+        <v>-0.218824225336559</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.03484385197524054</v>
+        <v>0.03486926252118899</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.03956764591523488</v>
+        <v>-0.03915802133205065</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1930856978917835</v>
+        <v>-0.1931068753440004</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9489109912643063</v>
+        <v>0.9489195226014283</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.05550683176122501</v>
+        <v>-0.05549788566449686</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1562047594022838</v>
+        <v>-0.1561456386271095</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.4898667658855189</v>
+        <v>-0.4892356764397228</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.1274711213086035</v>
+        <v>-0.1277065913529247</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.03767316999705252</v>
+        <v>-0.03738881415263039</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.09849784301137407</v>
+        <v>-0.09807475869789299</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.07583892624454303</v>
+        <v>-0.07554794405995992</v>
       </c>
     </row>
     <row r="8">
@@ -875,55 +875,55 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.0007965877032208406</v>
+        <v>-0.0007990859124778034</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0002284427686722433</v>
+        <v>-0.0002308575196248227</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0002345372470887257</v>
+        <v>0.0002323913823368846</v>
       </c>
       <c r="E8" t="n">
-        <v>8.903136686902814e-05</v>
+        <v>8.451679271108418e-05</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03485171557652254</v>
+        <v>0.03486044852935592</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03484385197524054</v>
+        <v>0.03486926252118899</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04569281333181557</v>
+        <v>0.04572593915546183</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.0190938074600693</v>
+        <v>-0.01910443812119384</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05652010621875398</v>
+        <v>0.05654142061270117</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.04570570055335551</v>
+        <v>-0.0457060209206458</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01227243494916291</v>
+        <v>0.01227609320113575</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.03354279519039434</v>
+        <v>-0.03347136095775486</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.031809528107053</v>
+        <v>-0.03184451706527877</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00346501097239451</v>
+        <v>0.003501428053857957</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.03669982041510728</v>
+        <v>-0.03663625454043101</v>
       </c>
       <c r="R8" t="n">
-        <v>0.04009018036427665</v>
+        <v>0.04010910537960239</v>
       </c>
     </row>
     <row r="9">
@@ -933,55 +933,55 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.001138456016208976</v>
+        <v>0.001177632623395438</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0003264826249559733</v>
+        <v>0.0003402204221353358</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0003351926459486996</v>
+        <v>-0.0003424809134566106</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0001272405974050862</v>
+        <v>-0.0001245544825252122</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06358113438030931</v>
+        <v>0.06371089685032538</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.03956764591523488</v>
+        <v>-0.03915802133205065</v>
       </c>
       <c r="H9" t="n">
-        <v>0.04569281333181557</v>
+        <v>0.04572593915546183</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.06501232434423686</v>
+        <v>-0.06501116173619884</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.04865895377470109</v>
+        <v>-0.04828296343645306</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.03445777626526311</v>
+        <v>-0.03433711244891577</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2649227337982176</v>
+        <v>0.2648506816746283</v>
       </c>
       <c r="N9" t="n">
-        <v>0.07479613036768749</v>
+        <v>0.07533673899990148</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.01823780746149687</v>
+        <v>-0.01887880047468948</v>
       </c>
       <c r="P9" t="n">
-        <v>0.243795101017428</v>
+        <v>0.2441026047930702</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.002721237223111839</v>
+        <v>-0.001727680259869888</v>
       </c>
       <c r="R9" t="n">
-        <v>0.5521370418046497</v>
+        <v>0.5525381600036388</v>
       </c>
     </row>
     <row r="10">
@@ -991,55 +991,55 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0004150461221734163</v>
+        <v>0.0004195049823813824</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001190255446989295</v>
+        <v>0.0001211958291220369</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0001222009510255731</v>
+        <v>-0.0001220010780195644</v>
       </c>
       <c r="E10" t="n">
-        <v>-4.638801656289278e-05</v>
+        <v>-4.436971680226623e-05</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2400588909222834</v>
+        <v>0.2400602062985029</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1930856978917835</v>
+        <v>-0.1931068753440004</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.0190938074600693</v>
+        <v>-0.01910443812119384</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.06501232434423686</v>
+        <v>-0.06501116173619884</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.1809334664453109</v>
+        <v>-0.1809546927560668</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1314165786600212</v>
+        <v>0.1314273997117306</v>
       </c>
       <c r="M10" t="n">
-        <v>0.4178876871456985</v>
+        <v>0.4178691396851781</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2173891530155526</v>
+        <v>0.2171975239587932</v>
       </c>
       <c r="O10" t="n">
-        <v>0.06949475834575224</v>
+        <v>0.06950850495401474</v>
       </c>
       <c r="P10" t="n">
-        <v>0.4606493185897083</v>
+        <v>0.4604969130392716</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.08550431892631789</v>
+        <v>-0.08562035705608291</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.04719311305969155</v>
+        <v>-0.04716179437360898</v>
       </c>
     </row>
     <row r="11">
@@ -1049,55 +1049,55 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.002190673373236816</v>
+        <v>-0.00219475635291615</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0006282340144309354</v>
+        <v>-0.000634069503543657</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000644994267613835</v>
+        <v>0.0006382823858887653</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0002448426507142497</v>
+        <v>0.0002321324463804022</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.2194922147890637</v>
+        <v>-0.2194358192293704</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9489109912643063</v>
+        <v>0.9489195226014283</v>
       </c>
       <c r="H11" t="n">
-        <v>0.05652010621875398</v>
+        <v>0.05654142061270117</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.04865895377470109</v>
+        <v>-0.04828296343645306</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1809334664453109</v>
+        <v>-0.1809546927560668</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.06658789565871483</v>
+        <v>-0.06657911034639749</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.1471246242895875</v>
+        <v>-0.1470732051773424</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.4925189215788677</v>
+        <v>-0.4919335190286616</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.1434908982023626</v>
+        <v>-0.1436981834542915</v>
       </c>
       <c r="P11" t="n">
-        <v>-0.02791193268459959</v>
+        <v>-0.02765637501747562</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.1007860048608157</v>
+        <v>-0.1004173198479076</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.08197594476044578</v>
+        <v>-0.08172527082725493</v>
       </c>
     </row>
     <row r="12">
@@ -1107,55 +1107,55 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.001168230183307748</v>
+        <v>-0.001166882514834089</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0003350211614406856</v>
+        <v>-0.0003371146942535636</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0003439589765832899</v>
+        <v>0.0003393545505090623</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000130568334932927</v>
+        <v>0.0001234174775012411</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02393631303165519</v>
+        <v>0.02395877534143304</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.05550683176122501</v>
+        <v>-0.05549788566449686</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.04570570055335551</v>
+        <v>-0.0457060209206458</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.03445777626526311</v>
+        <v>-0.03433711244891577</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1314165786600212</v>
+        <v>0.1314273997117306</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.06658789565871483</v>
+        <v>-0.06657911034639749</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1708513173075154</v>
+        <v>0.1708438506437887</v>
       </c>
       <c r="N12" t="n">
-        <v>0.02698329266492418</v>
+        <v>0.02695412148024802</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0448383772246024</v>
+        <v>-0.04488445878777349</v>
       </c>
       <c r="P12" t="n">
-        <v>0.09924788114610308</v>
+        <v>0.09922184575571608</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.03479393096904915</v>
+        <v>-0.03472797482349419</v>
       </c>
       <c r="R12" t="n">
-        <v>0.02005931371253081</v>
+        <v>0.02011168465698987</v>
       </c>
     </row>
     <row r="13">
@@ -1165,55 +1165,55 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.001626639367515433</v>
+        <v>0.001634561894822562</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0004664822206589636</v>
+        <v>0.0004722282032739412</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.0004789272012616987</v>
+        <v>-0.0004753657802256805</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.000181802864527671</v>
+        <v>-0.0001728824481591328</v>
       </c>
       <c r="F13" t="n">
-        <v>0.07430413120145614</v>
+        <v>0.07431340951733358</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1562047594022838</v>
+        <v>-0.1561456386271095</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01227243494916291</v>
+        <v>0.01227609320113575</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2649227337982176</v>
+        <v>0.2648506816746283</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4178876871456985</v>
+        <v>0.4178691396851781</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.1471246242895875</v>
+        <v>-0.1470732051773424</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1708513173075154</v>
+        <v>0.1708438506437887</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.141792868417497</v>
+        <v>0.1418231427009689</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0774226944066521</v>
+        <v>-0.07745542996770767</v>
       </c>
       <c r="P13" t="n">
-        <v>0.4082905838041766</v>
+        <v>0.4082729894982228</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.008730601160434332</v>
+        <v>0.008567290892541542</v>
       </c>
       <c r="R13" t="n">
-        <v>0.1356232885448407</v>
+        <v>0.1355845261914255</v>
       </c>
     </row>
     <row r="14">
@@ -1223,55 +1223,55 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0008292350778359623</v>
+        <v>0.0008368912573226979</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0002473712335797657</v>
+        <v>0.0002513753691377797</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0002559531140789645</v>
+        <v>-0.0002552659143308778</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0001022687416452939</v>
+        <v>-9.817768454003779e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4943070047759678</v>
+        <v>0.4941702061229365</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.4898667658855189</v>
+        <v>-0.4892356764397228</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.03354279519039434</v>
+        <v>-0.03347136095775486</v>
       </c>
       <c r="I14" t="n">
-        <v>0.07479613036768749</v>
+        <v>0.07533673899990148</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2173891530155526</v>
+        <v>0.2171975239587932</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.4925189215788677</v>
+        <v>-0.4919335190286616</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02698329266492418</v>
+        <v>0.02695412148024802</v>
       </c>
       <c r="M14" t="n">
-        <v>0.141792868417497</v>
+        <v>0.1418231427009689</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0.1019197545767987</v>
+        <v>0.1013953598326501</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0820351292776289</v>
+        <v>0.08252353942066859</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.08481109891317555</v>
+        <v>0.08541471848978671</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1443103067338433</v>
+        <v>0.1447960103534467</v>
       </c>
     </row>
     <row r="15">
@@ -1281,55 +1281,55 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001441381663814337</v>
+        <v>-0.001468032878502348</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.0006725001572570425</v>
+        <v>-0.000686895551804251</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0002627277026265624</v>
+        <v>0.0002627615482830759</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0003191134297649877</v>
+        <v>0.0003146591035266696</v>
       </c>
       <c r="F15" t="n">
-        <v>0.08673829665631627</v>
+        <v>0.08661242330160181</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.1274711213086035</v>
+        <v>-0.1277065913529247</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.031809528107053</v>
+        <v>-0.03184451706527877</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.01823780746149687</v>
+        <v>-0.01887880047468948</v>
       </c>
       <c r="J15" t="n">
-        <v>0.06949475834575224</v>
+        <v>0.06950850495401474</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.1434908982023626</v>
+        <v>-0.1436981834542915</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.0448383772246024</v>
+        <v>-0.04488445878777349</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.0774226944066521</v>
+        <v>-0.07745542996770767</v>
       </c>
       <c r="N15" t="n">
-        <v>0.1019197545767987</v>
+        <v>0.1013953598326501</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.1615960005312314</v>
+        <v>-0.1618807943276877</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0001096689255059679</v>
+        <v>-8.866174028652279e-05</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.0003305608357407635</v>
+        <v>-0.000304872512271589</v>
       </c>
     </row>
     <row r="16">
@@ -1339,55 +1339,55 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.001236075115874026</v>
+        <v>0.001248231948587792</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0003441936607030431</v>
+        <v>0.0003503091363556556</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0003448736322703561</v>
+        <v>-0.0003439280965548492</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.0001056255564091651</v>
+        <v>-9.939581574887584e-05</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.01866525350856984</v>
+        <v>-0.01860508477477728</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.03767316999705252</v>
+        <v>-0.03738881415263039</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00346501097239451</v>
+        <v>0.003501428053857957</v>
       </c>
       <c r="I16" t="n">
-        <v>0.243795101017428</v>
+        <v>0.2441026047930702</v>
       </c>
       <c r="J16" t="n">
-        <v>0.4606493185897083</v>
+        <v>0.4604969130392716</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.02791193268459959</v>
+        <v>-0.02765637501747562</v>
       </c>
       <c r="L16" t="n">
-        <v>0.09924788114610308</v>
+        <v>0.09922184575571608</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4082905838041766</v>
+        <v>0.4082729894982228</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0820351292776289</v>
+        <v>0.08252353942066859</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.1615960005312314</v>
+        <v>-0.1618807943276877</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>7.406795910534614e-05</v>
+        <v>5.94956240911887e-05</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.01592549486685088</v>
+        <v>-0.01560245657341144</v>
       </c>
     </row>
     <row r="17">
@@ -1397,55 +1397,55 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0001809993921905026</v>
+        <v>-0.0001451763067674667</v>
       </c>
       <c r="C17" t="n">
-        <v>-8.598931052432631e-05</v>
+        <v>-6.915549790652933e-05</v>
       </c>
       <c r="D17" t="n">
-        <v>3.049023167331969e-05</v>
+        <v>2.39965511444554e-05</v>
       </c>
       <c r="E17" t="n">
-        <v>3.100195286639313e-05</v>
+        <v>2.389315715687617e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01034470413893863</v>
+        <v>0.01058778278023932</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.09849784301137407</v>
+        <v>-0.09807475869789299</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.03669982041510728</v>
+        <v>-0.03663625454043101</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.002721237223111839</v>
+        <v>-0.001727680259869888</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.08550431892631789</v>
+        <v>-0.08562035705608291</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.1007860048608157</v>
+        <v>-0.1004173198479076</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.03479393096904915</v>
+        <v>-0.03472797482349419</v>
       </c>
       <c r="M17" t="n">
-        <v>0.008730601160434332</v>
+        <v>0.008567290892541542</v>
       </c>
       <c r="N17" t="n">
-        <v>0.08481109891317555</v>
+        <v>0.08541471848978671</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.0001096689255059679</v>
+        <v>-8.866174028652279e-05</v>
       </c>
       <c r="P17" t="n">
-        <v>7.406795910534614e-05</v>
+        <v>5.94956240911887e-05</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>0.05724434577987066</v>
+        <v>0.05815244118627622</v>
       </c>
     </row>
     <row r="18">
@@ -1455,52 +1455,52 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002490200880877209</v>
+        <v>0.002522203803982969</v>
       </c>
       <c r="C18" t="n">
-        <v>0.001249376620106088</v>
+        <v>0.001265568880261699</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2586872770139811</v>
+        <v>0.2585231779625458</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1147153398274242</v>
+        <v>0.1142621748737162</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2958933948009917</v>
+        <v>0.295895750700426</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.07583892624454303</v>
+        <v>-0.07554794405995992</v>
       </c>
       <c r="H18" t="n">
-        <v>0.04009018036427665</v>
+        <v>0.04010910537960239</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5521370418046497</v>
+        <v>0.5525381600036388</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.04719311305969155</v>
+        <v>-0.04716179437360898</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.08197594476044578</v>
+        <v>-0.08172527082725493</v>
       </c>
       <c r="L18" t="n">
-        <v>0.02005931371253081</v>
+        <v>0.02011168465698987</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1356232885448407</v>
+        <v>0.1355845261914255</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1443103067338433</v>
+        <v>0.1447960103534467</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.0003305608357407635</v>
+        <v>-0.000304872512271589</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.01592549486685088</v>
+        <v>-0.01560245657341144</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.05724434577987066</v>
+        <v>0.05815244118627622</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>

</xml_diff>